<commit_message>
Updating computational resources to reflect the scenarios
</commit_message>
<xml_diff>
--- a/docs/source/models/concept_models/vivarium_nutrition_optimization/kids/timestep scaling.xlsx
+++ b/docs/source/models/concept_models/vivarium_nutrition_optimization/kids/timestep scaling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibow\vivarium_research\docs\source\models\concept_models\vivarium_nutrition_optimization\kids\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lutzes\vivarium_research\docs\source\models\concept_models\vivarium_nutrition_optimization\kids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1F7A5BB-3384-4D5C-8D69-17AB768A5A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FE69A2-1198-49E7-B82D-F3AC1F2424FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="9765" xr2:uid="{87828C9E-A3A8-4731-A391-7D7FFCF86149}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{87828C9E-A3A8-4731-A391-7D7FFCF86149}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>hours</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>Full all.q cluster hours</t>
+  </si>
+  <si>
+    <t>Formula:</t>
   </si>
 </sst>
 </file>
@@ -634,19 +637,19 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.86328125" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" customWidth="1"/>
     <col min="2" max="2" width="24.6328125" customWidth="1"/>
-    <col min="3" max="3" width="9.6796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.76953125" customWidth="1"/>
-    <col min="10" max="10" width="14.6796875" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7265625" customWidth="1"/>
+    <col min="10" max="10" width="14.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -660,7 +663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>9</v>
       </c>
@@ -671,7 +674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -685,7 +688,7 @@
       <c r="I3" s="11"/>
       <c r="J3" s="12"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
@@ -700,7 +703,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>17</v>
       </c>
@@ -718,7 +721,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H6" s="7" t="s">
         <v>26</v>
       </c>
@@ -729,7 +732,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -737,22 +740,22 @@
         <v>8</v>
       </c>
       <c r="C7" s="1">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C8">
         <f>C7/365</f>
-        <v>1.0958904109589041E-2</v>
+        <v>7.6712328767123292E-2</v>
       </c>
       <c r="D8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -763,45 +766,52 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10">
         <f>C9/C8</f>
-        <v>456.25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.75">
+        <v>65.178571428571431</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="1">
         <v>19</v>
       </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
       <c r="E11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>16</v>
       </c>
       <c r="C12">
+        <f>219/3</f>
+        <v>73</v>
+      </c>
+      <c r="D12">
         <f>C11*C4+1</f>
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>17</v>
       </c>
       <c r="C13">
         <f>C10*C12</f>
-        <v>43800</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.75">
+        <v>4758.0357142857147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -810,10 +820,10 @@
       </c>
       <c r="C15">
         <f>C13+C5</f>
-        <v>44040</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.75">
+        <v>4998.0357142857147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>20</v>
       </c>
@@ -821,7 +831,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.75">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>19</v>
       </c>
@@ -829,7 +839,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.75">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
@@ -840,7 +850,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.75">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>3</v>
       </c>
@@ -854,43 +864,43 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.75">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>21</v>
       </c>
       <c r="C20">
         <f>C19*C15*C17*C16*C18</f>
-        <v>1268352000</v>
+        <v>143943428.5714286</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.75">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C21">
         <f>C20/60</f>
-        <v>21139200</v>
+        <v>2399057.1428571432</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="22" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C22">
         <f>C21/60</f>
-        <v>352320</v>
+        <v>39984.285714285717</v>
       </c>
       <c r="D22" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="30.25" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="23" spans="2:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="3">
         <f>C22/15000</f>
-        <v>23.488</v>
+        <v>2.6656190476190478</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
revert timestep scaling excel to intended version
</commit_message>
<xml_diff>
--- a/docs/source/models/concept_models/vivarium_nutrition_optimization/kids/timestep scaling.xlsx
+++ b/docs/source/models/concept_models/vivarium_nutrition_optimization/kids/timestep scaling.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibow\vivarium_research\docs\source\models\concept_models\vivarium_nutrition_optimization\kids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EC717A-201A-442A-ADF9-C3A82D30C1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1F7A5BB-3384-4D5C-8D69-17AB768A5A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="9765" xr2:uid="{87828C9E-A3A8-4731-A391-7D7FFCF86149}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>hours</t>
   </si>
@@ -113,31 +113,28 @@
     <t>total cluster time (across 15,000 threads)</t>
   </si>
   <si>
+    <t>Wave 1</t>
+  </si>
+  <si>
+    <t>Wave 2</t>
+  </si>
+  <si>
+    <t>9 for wave 1, 19 for wave 2</t>
+  </si>
+  <si>
     <t>1 for wave 1, 3 for wave 2</t>
   </si>
   <si>
+    <t>4 day timestep</t>
+  </si>
+  <si>
+    <t>28 day timestep</t>
+  </si>
+  <si>
     <t>From wasting paper test runs</t>
   </si>
   <si>
-    <t>JOBS</t>
-  </si>
-  <si>
-    <t>All locations</t>
-  </si>
-  <si>
-    <t>1 location</t>
-  </si>
-  <si>
-    <t>For one location/draw</t>
-  </si>
-  <si>
-    <t>For 5 draws/all locations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max workers=6000? </t>
-  </si>
-  <si>
-    <t>^Not all jobs will land at once</t>
+    <t>Full all.q cluster hours</t>
   </si>
 </sst>
 </file>
@@ -169,7 +166,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -214,11 +211,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -226,6 +303,20 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,7 +634,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -551,6 +642,8 @@
     <col min="1" max="1" width="18.86328125" customWidth="1"/>
     <col min="2" max="2" width="24.6328125" customWidth="1"/>
     <col min="3" max="3" width="9.6796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.76953125" customWidth="1"/>
+    <col min="10" max="10" width="14.6796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.75">
@@ -567,7 +660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:10" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="B2" t="s">
         <v>9</v>
       </c>
@@ -586,6 +679,11 @@
         <f>C2*C1</f>
         <v>48</v>
       </c>
+      <c r="H3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.75">
       <c r="B4" s="1" t="s">
@@ -594,6 +692,13 @@
       <c r="C4" s="1">
         <v>5</v>
       </c>
+      <c r="H4" s="5"/>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.75">
       <c r="B5" t="s">
@@ -603,10 +708,25 @@
         <f>C3*C4</f>
         <v>240</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="I6" s="1" t="s">
-        <v>27</v>
+      <c r="H5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5">
+        <v>3.8</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="H6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="8">
+        <v>23.5</v>
+      </c>
+      <c r="J6" s="9">
+        <v>3.5</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.75">
@@ -621,13 +741,6 @@
       </c>
       <c r="D7" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="I7" s="1">
-        <f>C16*C17*C18*C12</f>
-        <v>79200</v>
-      </c>
-      <c r="J7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.75">
@@ -638,13 +751,6 @@
       <c r="D8" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="1">
-        <f>I7/3</f>
-        <v>26400</v>
-      </c>
-      <c r="J8" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.75">
       <c r="B9" t="s">
@@ -656,13 +762,6 @@
       <c r="D9" t="s">
         <v>14</v>
       </c>
-      <c r="I9">
-        <f>I8/20</f>
-        <v>1320</v>
-      </c>
-      <c r="J9" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.75">
       <c r="B10" t="s">
@@ -678,14 +777,10 @@
         <v>15</v>
       </c>
       <c r="C11" s="1">
-        <v>13</v>
-      </c>
-      <c r="I11" s="1">
-        <f>I7/20*5</f>
-        <v>19800</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.75">
@@ -694,10 +789,7 @@
       </c>
       <c r="C12">
         <f>C11*C4+1</f>
-        <v>66</v>
-      </c>
-      <c r="J12" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.75">
@@ -706,10 +798,7 @@
       </c>
       <c r="C13">
         <f>C10*C12</f>
-        <v>30112.5</v>
-      </c>
-      <c r="J13" t="s">
-        <v>33</v>
+        <v>43800</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.75">
@@ -721,15 +810,15 @@
       </c>
       <c r="C15">
         <f>C13+C5</f>
-        <v>30352.5</v>
+        <v>44040</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="1">
-        <v>20</v>
+      <c r="C16">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.75">
@@ -737,7 +826,7 @@
         <v>19</v>
       </c>
       <c r="C17" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.75">
@@ -748,7 +837,7 @@
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.75">
@@ -762,7 +851,7 @@
         <v>4</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.75">
@@ -771,7 +860,7 @@
       </c>
       <c r="C20">
         <f>C19*C15*C17*C16*C18</f>
-        <v>1165536000</v>
+        <v>1268352000</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
@@ -780,7 +869,7 @@
     <row r="21" spans="2:5" x14ac:dyDescent="0.75">
       <c r="C21">
         <f>C20/60</f>
-        <v>19425600</v>
+        <v>21139200</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
@@ -789,7 +878,7 @@
     <row r="22" spans="2:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="C22">
         <f>C21/60</f>
-        <v>323760</v>
+        <v>352320</v>
       </c>
       <c r="D22" t="s">
         <v>0</v>
@@ -801,13 +890,16 @@
       </c>
       <c r="C23" s="3">
         <f>C22/15000</f>
-        <v>21.584</v>
+        <v>23.488</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H3:J3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>